<commit_message>
Fixed various issues for patch 3.11.07
</commit_message>
<xml_diff>
--- a/schedules/MMR.xlsx
+++ b/schedules/MMR.xlsx
@@ -5,25 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\forecast\forecaster2012\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\forecast\forecaster\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="354"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$J$88</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$J$89</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="76">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -474,14 +474,14 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1006,29 +1006,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J87"/>
+  <dimension ref="B1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="15.140625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="14.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="1" customWidth="1"/>
-    <col min="12" max="16" width="11.5703125" style="1"/>
-    <col min="17" max="17" width="6.28515625" style="1" customWidth="1"/>
-    <col min="18" max="22" width="11.5703125" style="1"/>
-    <col min="23" max="23" width="6.28515625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="3.28515625" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="1.5546875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.109375" style="1" customWidth="1"/>
+    <col min="8" max="10" width="14.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="1" customWidth="1"/>
+    <col min="12" max="16" width="11.5546875" style="1"/>
+    <col min="17" max="17" width="6.33203125" style="1" customWidth="1"/>
+    <col min="18" max="22" width="11.5546875" style="1"/>
+    <col min="23" max="23" width="6.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="3.33203125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1036,15 +1036,15 @@
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>11</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
@@ -1136,14 +1136,14 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="24" t="s">
+    <row r="8" spans="2:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="24"/>
       <c r="F8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1154,12 +1154,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="24"/>
-      <c r="C9" s="25" t="s">
+    <row r="9" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="25"/>
+      <c r="D9" s="24"/>
       <c r="F9" s="10" t="s">
         <v>1</v>
       </c>
@@ -1170,12 +1170,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="24"/>
-      <c r="C10" s="25" t="s">
+    <row r="10" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="24"/>
       <c r="F10" s="10" t="s">
         <v>11</v>
       </c>
@@ -1186,14 +1186,14 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="2:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="24"/>
       <c r="F11" s="10" t="s">
         <v>21</v>
       </c>
@@ -1204,19 +1204,19 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="F12" s="23" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="F12" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="2:10" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+    </row>
+    <row r="13" spans="2:10" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>72</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F14" s="10" t="s">
         <v>23</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F15" s="10" t="s">
         <v>24</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="26" t="s">
         <v>25</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
       <c r="F17" s="10" t="s">
@@ -1286,7 +1286,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F18" s="10" t="s">
         <v>27</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F19" s="13" t="s">
         <v>28</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F20" s="10" t="s">
         <v>29</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F21" s="10" t="s">
         <v>30</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F22" s="10" t="s">
         <v>31</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>32</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="15" t="s">
         <v>36</v>
       </c>
@@ -1366,15 +1366,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="23" t="s">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="16"/>
       <c r="C41" s="6" t="s">
         <v>39</v>
@@ -1386,7 +1386,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="17" t="s">
         <v>42</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="17" t="s">
         <v>44</v>
       </c>
@@ -1406,7 +1406,7 @@
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="17" t="s">
         <v>45</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="17" t="s">
         <v>47</v>
       </c>
@@ -1426,7 +1426,7 @@
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="17" t="s">
         <v>49</v>
       </c>
@@ -1436,7 +1436,7 @@
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="17" t="s">
         <v>51</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="17" t="s">
         <v>53</v>
       </c>
@@ -1456,14 +1456,14 @@
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B49" s="23" t="s">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
         <v>4</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>16</v>
       </c>
@@ -1491,7 +1491,7 @@
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>20</v>
       </c>
@@ -1502,14 +1502,14 @@
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B53" s="23" t="s">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>4</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>14</v>
       </c>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="E55" s="19"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
         <v>14</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="str">
         <f>D2</f>
         <v>Measles</v>
@@ -1558,7 +1558,7 @@
       <c r="D57" s="9"/>
       <c r="E57" s="19"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
         <v>72</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="17" t="s">
         <v>63</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="17" t="s">
         <v>64</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
         <v>32</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="15" t="s">
         <v>59</v>
       </c>
@@ -1606,15 +1606,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B65" s="23" t="s">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="23"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="23"/>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="16"/>
       <c r="C66" s="6" t="s">
         <v>39</v>
@@ -1626,7 +1626,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="17" t="s">
         <v>42</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="17" t="s">
         <v>44</v>
       </c>
@@ -1646,7 +1646,7 @@
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="17" t="s">
         <v>45</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="17" t="s">
         <v>47</v>
       </c>
@@ -1666,7 +1666,7 @@
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="17" t="s">
         <v>49</v>
       </c>
@@ -1677,7 +1677,7 @@
       <c r="E71" s="9"/>
       <c r="G71" s="20"/>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="17" t="s">
         <v>51</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="17" t="s">
         <v>53</v>
       </c>
@@ -1697,14 +1697,14 @@
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B74" s="23" t="s">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C74" s="25"/>
+      <c r="D74" s="25"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="6" t="s">
         <v>4</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
         <v>16</v>
       </c>
@@ -1732,7 +1732,7 @@
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="s">
         <v>20</v>
       </c>
@@ -1743,14 +1743,14 @@
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B78" s="23" t="s">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C78" s="23"/>
-      <c r="D78" s="23"/>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C78" s="25"/>
+      <c r="D78" s="25"/>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="6" t="s">
         <v>4</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="9" t="s">
         <v>14</v>
       </c>
@@ -1788,88 +1788,111 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D81" s="9"/>
       <c r="E81" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F81" s="19"/>
+        <v>62</v>
+      </c>
+      <c r="F81" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="G81" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E82" s="19"/>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="D82" s="9"/>
+      <c r="E82" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D83" s="9"/>
-      <c r="E83" s="19" t="s">
+      <c r="D83" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E83" s="19"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D84" s="9"/>
+      <c r="E84" s="19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B84" s="9" t="str">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="9" t="str">
         <f>$D$2</f>
         <v>Measles</v>
       </c>
-      <c r="C84" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D84" s="9"/>
-      <c r="E84" s="19"/>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B85" s="9" t="s">
-        <v>72</v>
-      </c>
       <c r="C85" s="9" t="s">
         <v>70</v>
       </c>
       <c r="D85" s="9"/>
-      <c r="E85" s="19" t="s">
+      <c r="E85" s="19"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D86" s="9"/>
+      <c r="E86" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B86" s="17" t="s">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C86" s="9">
+      <c r="C87" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B87" s="17" t="s">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C87" s="9">
+      <c r="C88" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="15">
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:D12"/>
     <mergeCell ref="F12:J12"/>
@@ -1880,11 +1903,6 @@
     <mergeCell ref="B53:D53"/>
     <mergeCell ref="B65:E65"/>
     <mergeCell ref="B74:D74"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1903,271 +1921,277 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A43"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A43"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection sqref="A1:A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.28515625" customWidth="1"/>
+    <col min="1" max="1" width="106.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
         <v>&lt;forecast seriesName="Measles"&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Measles" vaccineIds="158, 159, 1560, 160, 161"/&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B5&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C5&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Mumps" vaccineIds="158, 159, 1560, 162, 175"/&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Rubella" vaccineIds="158, 159, 1560, 160, 171, 175"/&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="MMRV" vaccineIds="159, 1560"/&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B8&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;IF(Schedules!D2="Measles",Schedules!C8,IF(Schedules!D2="Mumps",Schedules!C9,Schedules!C10))&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Same Live" vaccineIds="178, 162, 171, 175"/&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B11&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C11&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Other Live" vaccineIds="180, 2020, 1990, 1690, 1700, 210, 203"/&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B13&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C13&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Assume Comp" vaccineIds="-158"/&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B39&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C39&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D39&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E38&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="1 year"&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C60&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C59&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C42&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D42&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E42&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="1 year" interval="" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C43&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D43&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E43&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C44&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D44&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E44&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="12 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C45&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D45&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E45&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="16 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C46&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D46&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E46&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="50 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D47&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E47&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D48&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="str">
         <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B51&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C51&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D51&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E51&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!F51&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Same Live" afterInterval="4 weeks" age="" reason="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="str">
         <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B52&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C52&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D52&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E52&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!F52&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Other Live" afterInterval="4 weeks" age="" reason="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B55&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C55&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D55&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E55&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MMRV" schedule="P2" age="13 years" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B56&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C56&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D56&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E56&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MMRV" schedule="P2" age="" reason="MMRV should not be administered to persons 13 years of age or older."/&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B57&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C57&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D57&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E57&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Measles" schedule="P2" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B58&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C58&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D58&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E58&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Assume Comp" schedule="COMPLETE" age="" reason="Assuming adult received full MMR series as a child."/&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B64&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C64&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D64&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E63&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P2" dose="2" indication="" label="4-6 years"&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C87&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C88&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C87&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C67&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D67&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E67&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C68&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D68&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E68&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C69&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D69&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E69&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="4 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C70&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D70&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E70&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="7 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C71&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D71&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E71&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="50 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D72&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E72&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D73&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="str">
         <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B76&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C76&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D76&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E76&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!F76&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Same Live" afterInterval="4 weeks" age="" reason="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="str">
         <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B77&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C77&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D77&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E77&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!F77&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Other Live" afterInterval="4 weeks" age="" reason="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B80&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;" previousVaccineName="&amp;CHAR(34)&amp;Schedules!G80&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!F80&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MMRV" schedule="COMPLETE" age="13 years" reason="" previousVaccineName="MMRV" minInterval="4 weeks"/&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B81&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;" previousVaccineName="&amp;CHAR(34)&amp;Schedules!G81&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!F81&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MMRV" schedule="INVALID" age="" reason="MMRV must be administered no sooner than 4 weeks after previous MMRV." previousVaccineName="MMRV" minInterval=""/&gt;</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">    &lt;indicate vaccineName="MMRV" schedule="COMPLETE" age="" reason="MMRV should not be administered to persons 13 years of age or older." previousVaccineName="MMRV" minInterval="4 weeks"/&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B82&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;" previousVaccineName="&amp;CHAR(34)&amp;Schedules!G82&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!F82&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="MMRV" schedule="INVALID" age="" reason="MMRV must be administered no sooner than 4 weeks after previous MMRV." previousVaccineName="MMRV" minInterval=""/&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B83&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;" previousVaccineName="&amp;CHAR(34)&amp;Schedules!G83&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!F83&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MMRV" schedule="COMPLETE" age="13 years" reason="" previousVaccineName="" minInterval=""/&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="22" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B83&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;" previousVaccineName="&amp;CHAR(34)&amp;Schedules!G82&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!F82&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MMRV" schedule="COMPLETE" age="" reason="MMRV should not be administered to persons 13 years of age or older." previousVaccineName="" minInterval=""/&gt;</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B84&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;" previousVaccineName="&amp;CHAR(34)&amp;Schedules!G84&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!F84&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="Measles" schedule="COMPLETE" age="" reason="" previousVaccineName="" minInterval=""/&gt;</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">    &lt;indicate vaccineName="MMRV" schedule="COMPLETE" age="" reason="MMRV should not be administered to persons 13 years of age or older." previousVaccineName="" minInterval=""/&gt;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B85&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C85&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;" previousVaccineName="&amp;CHAR(34)&amp;Schedules!G85&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!F85&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="Measles" schedule="COMPLETE" age="" reason="" previousVaccineName="" minInterval=""/&gt;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B86&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;" previousVaccineName="&amp;CHAR(34)&amp;Schedules!G86&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!F86&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Assume Comp" schedule="COMPLETE" age="" reason="Assuming adult received full MMR series as a child." previousVaccineName="" minInterval=""/&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="22" t="str">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="22" t="str">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="str">
         <f>"&lt;/forecast&gt;"</f>
         <v>&lt;/forecast&gt;</v>
       </c>

</xml_diff>